<commit_message>
Agregando el algoritmo para get y remove
</commit_message>
<xml_diff>
--- a/equipos.xlsx
+++ b/equipos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\Documents\Academlo\algoritmos-estructuras3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D75DB9E-00A7-4007-8CBA-E843C5FEB92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5233C77-51E0-4D31-A5C2-BAE41D1CFE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{A40F6413-EF04-4757-BCCB-69FBF7DEDADC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Grupo 1</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>Jose Gregorio Palacio</t>
+  </si>
+  <si>
+    <t>Marlene Villalobos</t>
   </si>
 </sst>
 </file>
@@ -264,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -296,11 +299,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -325,6 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C002411-3B76-49BA-B062-D0ED28322279}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,9 +743,6 @@
       <c r="B4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" s="12" t="s">
         <v>15</v>
       </c>
@@ -804,9 +816,6 @@
       <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="C10" s="8" t="s">
         <v>39</v>
       </c>
@@ -902,6 +911,21 @@
         <v>37</v>
       </c>
     </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E24" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E25" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E26" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>